<commit_message>
Add the gage area to COMID drainage area factors for Breitenbush and Boulder Creek. Flow.xml - Increase the Breitenbush spring from 20 cfs to 30 cfs. HBV.csv - Decrease ET_MULT for Blowout51 from 6.46036 to 2.0. FLOWreports_NSantiam.xml - Add the gage area to COMID drainage area factors for Boulder Creek and Breitenbush. Flow.cpp - Stand up the calculation of the CUM_ALREA attributes, by moving the call to PopulateCatchmentCumulativeAreas() to after the call to SetAllCatchmentAttributes() (which is where pCatchment->m_area gets initialized).
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\NSantiam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9C03A4-2EC5-40C7-9F8D-7B92E51AEB08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAFD6B5-4209-44F3-89B9-1E6324D8AF5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +739,7 @@
         <v>283576000</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10:E13" si="0">D10/1000000</f>
+        <f t="shared" ref="E10:E16" si="0">D10/1000000</f>
         <v>283.57600000000002</v>
       </c>
       <c r="F10">
@@ -959,6 +959,13 @@
       <c r="C15">
         <v>23780701</v>
       </c>
+      <c r="D15" s="2">
+        <v>273121248</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>273.12124799999998</v>
+      </c>
       <c r="F15">
         <v>14179000</v>
       </c>
@@ -993,6 +1000,10 @@
         <f t="shared" si="1"/>
         <v>279.71871587999999</v>
       </c>
+      <c r="Q15">
+        <f>P15/E15</f>
+        <v>1.0241558206412413</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1001,6 +1012,13 @@
       <c r="C16">
         <v>23780591</v>
       </c>
+      <c r="D16" s="2">
+        <v>557769920</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>557.76991999999996</v>
+      </c>
       <c r="F16">
         <v>14178000</v>
       </c>
@@ -1034,6 +1052,10 @@
       <c r="P16" s="4">
         <f t="shared" si="1"/>
         <v>559.43743175999998</v>
+      </c>
+      <c r="Q16">
+        <f>P16/E16</f>
+        <v>1.0029896050328422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Do new spinups for PEST_Blowout51 and PEST_LittleNSantiam50. PEST_Blowout51/flow2020.ic, HRU_PEST_Blowout51.dbf, IDU_PEST_Blowout51.dbf, Reach_PEST_Blowout51.dbf - from spinup over 2000-09. PEST_LittleNSantiam50/flow2010.ic, HRU_PEST_LittleNSantiam50.dbf, IDU_PEST_LittleNSantiam50.dbf, Reach_PEST_LittleNSantiam50.dbf - from spinup over 2000-09.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\NSantiam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E59752-699D-4AA0-8658-5386326166A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F791341-409D-4109-805E-2147AF73E146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Nsantiam HBVCALIB and gages</t>
   </si>
@@ -88,9 +88,6 @@
     <t>DET = DET12 + Blowout51</t>
   </si>
   <si>
-    <t>Mehama = Mehama37 + DET12 + Blowout51</t>
-  </si>
-  <si>
     <t>LittleNSantiam50 and Blowout51 are complete watersheds.</t>
   </si>
   <si>
@@ -203,6 +200,12 @@
   </si>
   <si>
     <t>Nsantiam</t>
+  </si>
+  <si>
+    <t>Mehama = Mehama37 + DET12 + Blowout51 + LittleNSantiam50</t>
+  </si>
+  <si>
+    <t>LowerNSantiam44 is also called GreensBr44 sometimes.</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED544CC-C2DF-41BC-A13B-027C1D733E2A}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,486 +602,491 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>23780877</v>
+      </c>
+      <c r="D10" s="2">
+        <v>197520000</v>
+      </c>
+      <c r="E10" s="4">
+        <f>D10/1000000</f>
+        <v>197.52</v>
+      </c>
+      <c r="F10">
+        <v>14184100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>240</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10">
+        <v>502244</v>
+      </c>
+      <c r="M10">
+        <v>4950520</v>
+      </c>
+      <c r="N10">
+        <v>23780883</v>
+      </c>
+      <c r="O10">
+        <v>736</v>
+      </c>
+      <c r="P10" s="4">
+        <f>O10*2.58998811</f>
+        <v>1906.2312489600001</v>
+      </c>
+      <c r="Q10">
+        <f>P10/(SUM(E10:E14))</f>
+        <v>0.99903978503020396</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>23780481</v>
+      </c>
+      <c r="D11" s="2">
+        <v>283576000</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" ref="E11:E19" si="0">D11/1000000</f>
+        <v>283.57600000000002</v>
+      </c>
+      <c r="F11">
+        <v>14183000</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H11">
+        <v>602.49</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>530257</v>
+      </c>
+      <c r="M11">
+        <v>4959601</v>
+      </c>
+      <c r="N11">
+        <v>23780481</v>
+      </c>
+      <c r="O11">
+        <v>654.35</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" ref="P11:P19" si="1">O11*2.58998811</f>
+        <v>1694.7587197785001</v>
+      </c>
+      <c r="Q11">
+        <f>P11/(E11+E12+E14)</f>
+        <v>1.1948262227022655</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>23780877</v>
-      </c>
-      <c r="D9" s="2">
-        <v>197520000</v>
-      </c>
-      <c r="E9" s="4">
-        <f>D9/1000000</f>
-        <v>197.52</v>
-      </c>
-      <c r="F9">
-        <v>14184100</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9">
-        <v>240</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9">
-        <v>502244</v>
-      </c>
-      <c r="M9">
-        <v>4950520</v>
-      </c>
-      <c r="N9">
-        <v>23780883</v>
-      </c>
-      <c r="O9">
-        <v>736</v>
-      </c>
-      <c r="P9" s="4">
-        <f>O9*2.58998811</f>
-        <v>1906.2312489600001</v>
-      </c>
-      <c r="Q9">
-        <f>P9/(SUM(E9:E13))</f>
-        <v>0.99903978503020396</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>23780481</v>
-      </c>
-      <c r="D10" s="2">
-        <v>283576000</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" ref="E10:E18" si="0">D10/1000000</f>
-        <v>283.57600000000002</v>
-      </c>
-      <c r="F10">
-        <v>14183000</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10">
-        <v>602.49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10">
-        <v>530257</v>
-      </c>
-      <c r="M10">
-        <v>4959601</v>
-      </c>
-      <c r="N10">
-        <v>23780481</v>
-      </c>
-      <c r="O10">
-        <v>654.35</v>
-      </c>
-      <c r="P10" s="4">
-        <f t="shared" ref="P10:P18" si="1">O10*2.58998811</f>
-        <v>1694.7587197785001</v>
-      </c>
-      <c r="Q10">
-        <f>P10/(E10+E11+E13)</f>
-        <v>1.1948262227022655</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>23780511</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>1068300000</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
         <v>1068.3</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>14181500</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12">
+        <v>1093.78</v>
+      </c>
+      <c r="I12" t="s">
         <v>35</v>
       </c>
-      <c r="H11">
-        <v>1093.78</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J12" t="s">
         <v>36</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K12" t="s">
         <v>37</v>
       </c>
-      <c r="K11" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11">
+      <c r="L12">
         <v>555609</v>
       </c>
-      <c r="M11">
+      <c r="M12">
         <v>4955839</v>
       </c>
-      <c r="N11">
+      <c r="N12">
         <v>23780511</v>
       </c>
-      <c r="O11">
+      <c r="O12">
         <v>453</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P12" s="4">
         <f t="shared" si="1"/>
         <v>1173.2646138300001</v>
       </c>
-      <c r="Q11">
-        <f>P11/(E11+E13)</f>
+      <c r="Q12">
+        <f>P12/(E12+E14)</f>
         <v>1.0338605160258942</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>23780805</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <v>292129000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>292.12900000000002</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>14182500</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13">
+        <v>655.41</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
         <v>41</v>
       </c>
-      <c r="H12">
-        <v>655.41</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K13" t="s">
         <v>42</v>
       </c>
-      <c r="K12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12">
+      <c r="L13">
         <v>533398</v>
       </c>
-      <c r="M12">
+      <c r="M13">
         <v>4959894</v>
       </c>
-      <c r="N12">
+      <c r="N13">
         <v>23780805</v>
       </c>
-      <c r="O12">
+      <c r="O13">
         <v>112</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P13" s="4">
         <f t="shared" si="1"/>
         <v>290.07866832000002</v>
       </c>
-      <c r="Q12">
-        <f>P12/E12</f>
+      <c r="Q13">
+        <f>P13/E13</f>
         <v>0.99298141683982077</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>23780557</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <v>66538400</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E14" s="4">
         <f t="shared" si="0"/>
         <v>66.538399999999996</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>14180300</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14">
+        <v>1840</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
         <v>44</v>
       </c>
-      <c r="H13">
-        <v>1840</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K14" t="s">
         <v>45</v>
       </c>
-      <c r="K13" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13">
+      <c r="L14">
         <v>569004</v>
       </c>
-      <c r="M13">
+      <c r="M14">
         <v>4944779</v>
       </c>
-      <c r="N13">
+      <c r="N14">
         <v>23780557</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O14" s="5">
         <v>26</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P14" s="4">
         <f t="shared" si="1"/>
         <v>67.339690860000005</v>
       </c>
-      <c r="Q13">
-        <f>P13/E13</f>
+      <c r="Q14">
+        <f>P14/E14</f>
         <v>1.0120425327329783</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2">
-        <f>SUM(D9:D13)</f>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2">
+        <f>SUM(D10:D14)</f>
         <v>1908063400</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>1908.0634</v>
       </c>
-      <c r="O14" s="5"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E15" s="4"/>
       <c r="O15" s="5"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E16" s="4"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
         <v>23780701</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>273121248</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="4">
         <f t="shared" si="0"/>
         <v>273.12124799999998</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>14179000</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18">
+        <v>1573.95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" t="s">
         <v>49</v>
       </c>
-      <c r="H17">
-        <v>1573.95</v>
-      </c>
-      <c r="I17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K18" t="s">
         <v>50</v>
       </c>
-      <c r="K17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L17">
+      <c r="L18">
         <v>569039</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>4955858</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>23780701</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>108</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P18" s="4">
         <f t="shared" si="1"/>
         <v>279.71871587999999</v>
       </c>
-      <c r="Q17">
-        <f>P17/E17</f>
+      <c r="Q18">
+        <f>P18/E18</f>
         <v>1.0241558206412413</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19">
         <v>23780591</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>557769920</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E19" s="4">
         <f t="shared" si="0"/>
         <v>557.76991999999996</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>14178000</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19">
+        <v>1590.07</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
         <v>52</v>
       </c>
-      <c r="H18">
-        <v>1590.07</v>
-      </c>
-      <c r="I18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K19" t="s">
         <v>53</v>
       </c>
-      <c r="K18" t="s">
-        <v>54</v>
-      </c>
-      <c r="L18">
+      <c r="L19">
         <v>571294</v>
       </c>
-      <c r="M18">
+      <c r="M19">
         <v>4950790</v>
       </c>
-      <c r="N18">
+      <c r="N19">
         <v>23780591</v>
       </c>
-      <c r="O18">
+      <c r="O19">
         <v>216</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P19" s="4">
         <f t="shared" si="1"/>
         <v>559.43743175999998</v>
       </c>
-      <c r="Q18">
-        <f>P18/E18</f>
+      <c r="Q19">
+        <f>P19/E19</f>
         <v>1.0029896050328422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit David Holman's new HBV calibration parameter values for the North Santiam. HBV.csv - New parameter values for Mehama37 and GreensBr44 (aka LowerNSantiam44), obtained from PEST runs. HBV_OUWIN.csv - Delete as unwanted. FLOWreports_PEST_Mehama37.xml - Add columns to the monthly Q_DISCHARG report for all the gages in the Mehama drainage. Flow.cpp - Add an error check to prevent a crash when the HBV CSV file is open in Excel.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/NSantiam/HBVCALIBandGages_NSantiam.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\NSantiam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F791341-409D-4109-805E-2147AF73E146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC81FF9A-EEB1-42FF-A468-B2E908A0905A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{05AF46A7-1955-4C81-B6D9-039282A25E35}"/>
   </bookViews>
@@ -573,59 +573,59 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
-    <col min="18" max="18" width="33.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="33.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -678,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>44</v>
       </c>
@@ -737,7 +737,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>37</v>
       </c>
@@ -796,7 +796,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -852,7 +852,7 @@
         <v>1.0338605160258942</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -908,7 +908,7 @@
         <v>0.99298141683982077</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51</v>
       </c>
@@ -964,7 +964,7 @@
         <v>1.0120425327329783</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>54</v>
       </c>
@@ -979,12 +979,12 @@
       <c r="O15" s="5"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E16" s="4"/>
       <c r="O16" s="5"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>46</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>1.0241558206412413</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>

</xml_diff>